<commit_message>
Fixed images with alt text
</commit_message>
<xml_diff>
--- a/chapters.xlsx
+++ b/chapters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10650"/>
   </bookViews>
   <sheets>
     <sheet name="chapters" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="97">
   <si>
     <t>1.03.IntroductionToWorkbench.md</t>
   </si>
@@ -67,18 +67,6 @@
     <t>destination</t>
   </si>
   <si>
-    <t>source folder</t>
-  </si>
-  <si>
-    <t>source file</t>
-  </si>
-  <si>
-    <t>destination folder</t>
-  </si>
-  <si>
-    <t>destination file</t>
-  </si>
-  <si>
     <t>DesktopBasic1Basics</t>
   </si>
   <si>
@@ -235,9 +223,6 @@
     <t>2.Exercise6.md</t>
   </si>
   <si>
-    <t>chap</t>
-  </si>
-  <si>
     <t>file</t>
   </si>
   <si>
@@ -262,9 +247,6 @@
     <t>CourseResources</t>
   </si>
   <si>
-    <t>WhyFME</t>
-  </si>
-  <si>
     <t>Lecture</t>
   </si>
   <si>
@@ -314,6 +296,21 @@
   </si>
   <si>
     <t>indent</t>
+  </si>
+  <si>
+    <t>chapter</t>
+  </si>
+  <si>
+    <t>source_folder</t>
+  </si>
+  <si>
+    <t>source_file</t>
+  </si>
+  <si>
+    <t>destination_folder</t>
+  </si>
+  <si>
+    <t>destination_file</t>
   </si>
 </sst>
 </file>
@@ -1122,11 +1119,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J57"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1141,25 +1136,25 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
@@ -1171,7 +1166,7 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -1180,10 +1175,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G2" s="2" t="str">
         <f>IF(ISBLANK(A2),C2&amp;"."&amp;E2&amp;"."&amp;B2&amp;".md",C2&amp;"."&amp;E2&amp;"."&amp;RIGHT(B2,LEN(B2)-5))</f>
@@ -1201,49 +1196,49 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G3" s="2" t="str">
-        <f t="shared" ref="G3:G38" si="0">IF(ISBLANK(A3),C3&amp;"."&amp;E3&amp;"."&amp;B3&amp;".md",C3&amp;"."&amp;E3&amp;"."&amp;RIGHT(B3,LEN(B3)-5))</f>
+        <f t="shared" ref="G3:G37" si="0">IF(ISBLANK(A3),C3&amp;"."&amp;E3&amp;"."&amp;B3&amp;".md",C3&amp;"."&amp;E3&amp;"."&amp;RIGHT(B3,LEN(B3)-5))</f>
         <v>0.01.CourseOverview.md</v>
       </c>
       <c r="H3" s="2" t="str">
-        <f t="shared" ref="H3:H57" si="1">IF(ISBLANK(A3),"",A3&amp;"/"&amp;B3)</f>
+        <f t="shared" ref="H3:H56" si="1">IF(ISBLANK(A3),"",A3&amp;"/"&amp;B3)</f>
         <v/>
       </c>
       <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I57" si="2">F3&amp;"/"&amp;G3</f>
+        <f t="shared" ref="I3:I56" si="2">F3&amp;"/"&amp;G3</f>
         <v>CADGIS0About/0.01.CourseOverview.md</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1261,45 +1256,45 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>1.00.Lecture.md</v>
       </c>
       <c r="I5" s="2" t="str">
-        <f>F5&amp;"/"&amp;G5</f>
+        <f t="shared" si="2"/>
         <v>CADGIS1Lecture/1.00.Lecture.md</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1309,981 +1304,984 @@
         <f>IF(ISBLANK(A6),"",A6&amp;"/"&amp;B5)</f>
         <v/>
       </c>
+      <c r="I6" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>CADGIS1Lecture/1.01.DataIntegration.md</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1.02.WhyFME.md</v>
+        <v>1.02.WhatIsFME.md</v>
       </c>
       <c r="H7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>DesktopBasic1Basics/1.01.WhatIsFME.md</v>
       </c>
       <c r="I7" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS1Lecture/1.02.WhyFME.md</v>
+        <v>CADGIS1Lecture/1.02.WhatIsFME.md</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1.03.WhatIsFME.md</v>
+        <v>1.03.DataTransformation.md</v>
       </c>
       <c r="H8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.01.WhatIsFME.md</v>
+        <v>DesktopBasic2Transformation/2.00.DataTransformation.md</v>
       </c>
       <c r="I8" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS1Lecture/1.03.WhatIsFME.md</v>
+        <v>CADGIS1Lecture/1.03.DataTransformation.md</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1.04.DataTransformation.md</v>
+        <v>1.04.WhatIsDataTransformation.md</v>
       </c>
       <c r="H9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.00.DataTransformation.md</v>
+        <v>DesktopBasic2Transformation/2.01.WhatIsDataTransformation.md</v>
       </c>
       <c r="I9" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS1Lecture/1.04.DataTransformation.md</v>
+        <v>CADGIS1Lecture/1.04.WhatIsDataTransformation.md</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1.05.WhatIsDataTransformation.md</v>
+        <v>1.05.StructuralTransformation.md</v>
       </c>
       <c r="H10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.01.WhatIsDataTransformation.md</v>
+        <v>DesktopBasic2Transformation/2.02.StructuralTransformation.md</v>
       </c>
       <c r="I10" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS1Lecture/1.05.WhatIsDataTransformation.md</v>
+        <v>CADGIS1Lecture/1.05.StructuralTransformation.md</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1.06.StructuralTransformation.md</v>
+        <v>1.06.SchemaEditing.md</v>
       </c>
       <c r="H11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.02.StructuralTransformation.md</v>
+        <v>DesktopBasic2Transformation/2.03.SchemaEditing.md</v>
       </c>
       <c r="I11" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS1Lecture/1.06.StructuralTransformation.md</v>
+        <v>CADGIS1Lecture/1.06.SchemaEditing.md</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1.07.SchemaEditing.md</v>
+        <v>1.07.SchemaMapping.md</v>
       </c>
       <c r="H12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.03.SchemaEditing.md</v>
+        <v>DesktopBasic2Transformation/2.04.SchemaMapping.md</v>
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS1Lecture/1.07.SchemaEditing.md</v>
+        <v>CADGIS1Lecture/1.07.SchemaMapping.md</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>54</v>
-      </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="G13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1.08.SchemaMapping.md</v>
+        <v>2.00.LabDemonstration.md</v>
       </c>
       <c r="H13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.04.SchemaMapping.md</v>
+        <v/>
       </c>
       <c r="I13" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS1Lecture/1.08.SchemaMapping.md</v>
+        <v>CADGIS2LabDemonstration/2.00.LabDemonstration.md</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>90</v>
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.00.LabDemonstration.md</v>
+        <v>2.01.FMEDesktopComponents.md</v>
       </c>
       <c r="H14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>DesktopBasic1Basics/1.02.FMEDesktopComponents.md</v>
       </c>
       <c r="I14" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.00.LabDemonstration.md</v>
+        <v>CADGIS2LabDemonstration/2.01.FMEDesktopComponents.md</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.01.FMEDesktopComponents.md</v>
+        <v>2.02.IntroductionToWorkbench.md</v>
       </c>
       <c r="H15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.02.FMEDesktopComponents.md</v>
+        <v>DesktopBasic1Basics/1.03.IntroductionToWorkbench.md</v>
       </c>
       <c r="I15" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.01.FMEDesktopComponents.md</v>
+        <v>CADGIS2LabDemonstration/2.02.IntroductionToWorkbench.md</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.02.IntroductionToWorkbench.md</v>
+        <v>2.03.WindowControl.md</v>
       </c>
       <c r="H16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.03.IntroductionToWorkbench.md</v>
+        <v>DesktopBasic1Basics/1.04.WindowControl.md</v>
       </c>
       <c r="I16" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.02.IntroductionToWorkbench.md</v>
+        <v>CADGIS2LabDemonstration/2.03.WindowControl.md</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.03.WindowControl.md</v>
+        <v>2.04.CreatingATranslation.md</v>
       </c>
       <c r="H17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.04.WindowControl.md</v>
+        <v>DesktopBasic1Basics/1.05.CreatingATranslation.md</v>
       </c>
       <c r="I17" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.03.WindowControl.md</v>
+        <v>CADGIS2LabDemonstration/2.04.CreatingATranslation.md</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.04.CreatingATranslation.md</v>
+        <v>2.05.TheNewWorkspace.md</v>
       </c>
       <c r="H18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.05.CreatingATranslation.md</v>
+        <v>DesktopBasic1Basics/1.06.TheNewWorkspace.md</v>
       </c>
       <c r="I18" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.04.CreatingATranslation.md</v>
+        <v>CADGIS2LabDemonstration/2.05.TheNewWorkspace.md</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.05.TheNewWorkspace.md</v>
+        <v>2.06.RunningTheWorkspace.md</v>
       </c>
       <c r="H19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.06.TheNewWorkspace.md</v>
+        <v>DesktopBasic1Basics/1.07.RunningTheWorkspace.md</v>
       </c>
       <c r="I19" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.05.TheNewWorkspace.md</v>
+        <v>CADGIS2LabDemonstration/2.06.RunningTheWorkspace.md</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.06.RunningTheWorkspace.md</v>
+        <v>2.07.WhatIsDataInspection.md</v>
       </c>
       <c r="H20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.07.RunningTheWorkspace.md</v>
+        <v>DesktopBasic1Basics/1.08.WhatIsDataInspection.md</v>
       </c>
       <c r="I20" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.06.RunningTheWorkspace.md</v>
+        <v>CADGIS2LabDemonstration/2.07.WhatIsDataInspection.md</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.07.WhatIsDataInspection.md</v>
+        <v>2.08.IntroductionToDataInspector.md</v>
       </c>
       <c r="H21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.08.WhatIsDataInspection.md</v>
+        <v>DesktopBasic1Basics/1.09.IntroductionToDataInspector.md</v>
       </c>
       <c r="I21" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.07.WhatIsDataInspection.md</v>
+        <v>CADGIS2LabDemonstration/2.08.IntroductionToDataInspector.md</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.08.IntroductionToDataInspector.md</v>
+        <v>2.09.ViewingData.md</v>
       </c>
       <c r="H22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.09.IntroductionToDataInspector.md</v>
+        <v>DesktopBasic1Basics/1.10.ViewingData.md</v>
       </c>
       <c r="I22" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.08.IntroductionToDataInspector.md</v>
+        <v>CADGIS2LabDemonstration/2.09.ViewingData.md</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.09.ViewingData.md</v>
+        <v>2.10.QueryingData.md</v>
       </c>
       <c r="H23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.10.ViewingData.md</v>
+        <v>DesktopBasic1Basics/1.11.QueryingData.md</v>
       </c>
       <c r="I23" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.09.ViewingData.md</v>
+        <v>CADGIS2LabDemonstration/2.10.QueryingData.md</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.10.QueryingData.md</v>
+        <v>2.11.DataInspectorDisplayControl.md</v>
       </c>
       <c r="H24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.11.QueryingData.md</v>
+        <v>DesktopBasic1Basics/1.12.DataInspectorDisplayControl.md</v>
       </c>
       <c r="I24" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.10.QueryingData.md</v>
+        <v>CADGIS2LabDemonstration/2.11.DataInspectorDisplayControl.md</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.11.DataInspectorDisplayControl.md</v>
+        <v>2.12.BackgroundMaps.md</v>
       </c>
       <c r="H25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.12.DataInspectorDisplayControl.md</v>
+        <v>DesktopBasic1Basics/1.13.BackgroundMaps.md</v>
       </c>
       <c r="I25" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.11.DataInspectorDisplayControl.md</v>
+        <v>CADGIS2LabDemonstration/2.12.BackgroundMaps.md</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.12.BackgroundMaps.md</v>
+        <v>2.13.ReaderParameters.md</v>
       </c>
       <c r="H26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.13.BackgroundMaps.md</v>
+        <v>DesktopBasic1Basics/1.14.ReaderParameters.md</v>
       </c>
       <c r="I26" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.12.BackgroundMaps.md</v>
+        <v>CADGIS2LabDemonstration/2.13.ReaderParameters.md</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.13.ReaderParameters.md</v>
+        <v>2.14.WriterParameters.md</v>
       </c>
       <c r="H27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.14.ReaderParameters.md</v>
+        <v>DesktopBasic1Basics/1.15.WriterParameters.md</v>
       </c>
       <c r="I27" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.13.ReaderParameters.md</v>
+        <v>CADGIS2LabDemonstration/2.14.WriterParameters.md</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>12</v>
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.14.WriterParameters.md</v>
+        <v>2.15.TransformationWithTransformers.md</v>
       </c>
       <c r="H28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.15.WriterParameters.md</v>
+        <v>DesktopBasic2Transformation/2.05.TransformationWithTransformers.md</v>
       </c>
       <c r="I28" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.14.WriterParameters.md</v>
+        <v>CADGIS2LabDemonstration/2.15.TransformationWithTransformers.md</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.15.TransformationWithTransformers.md</v>
+        <v>2.16.ContentTransformation.md</v>
       </c>
       <c r="H29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.05.TransformationWithTransformers.md</v>
+        <v>DesktopBasic2Transformation/2.06.ContentTransformation.md</v>
       </c>
       <c r="I29" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.15.TransformationWithTransformers.md</v>
+        <v>CADGIS2LabDemonstration/2.16.ContentTransformation.md</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.16.ContentTransformation.md</v>
+        <v>2.17.TransformersInSeries.md</v>
       </c>
       <c r="H30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.06.ContentTransformation.md</v>
+        <v>DesktopBasic2Transformation/2.07.TransformersInSeries.md</v>
       </c>
       <c r="I30" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.16.ContentTransformation.md</v>
+        <v>CADGIS2LabDemonstration/2.17.TransformersInSeries.md</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.17.TransformersInSeries.md</v>
+        <v>2.18.FeatureCounts.md</v>
       </c>
       <c r="H31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.07.TransformersInSeries.md</v>
+        <v>DesktopBasic2Transformation/2.08.FeatureCounts.md</v>
       </c>
       <c r="I31" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.17.TransformersInSeries.md</v>
+        <v>CADGIS2LabDemonstration/2.18.FeatureCounts.md</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B32" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.18.FeatureCounts.md</v>
+        <v>2.19.TransformersInParallel.md</v>
       </c>
       <c r="H32" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.08.FeatureCounts.md</v>
+        <v>DesktopBasic2Transformation/2.09.TransformersInParallel.md</v>
       </c>
       <c r="I32" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.18.FeatureCounts.md</v>
+        <v>CADGIS2LabDemonstration/2.19.TransformersInParallel.md</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G33" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.19.TransformersInParallel.md</v>
+        <v>2.20.GroupByProcessing.md</v>
       </c>
       <c r="H33" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.09.TransformersInParallel.md</v>
+        <v>DesktopBasic2Transformation/2.10.GroupByProcessing.md</v>
       </c>
       <c r="I33" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.19.TransformersInParallel.md</v>
+        <v>CADGIS2LabDemonstration/2.20.GroupByProcessing.md</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G34" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.20.GroupByProcessing.md</v>
+        <v>2.21.DataInspectionFromWorkbench.md</v>
       </c>
       <c r="H34" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.10.GroupByProcessing.md</v>
+        <v>DesktopBasic2Transformation/2.11.DataInspectionFromWorkbench.md</v>
       </c>
       <c r="I34" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.20.GroupByProcessing.md</v>
+        <v>CADGIS2LabDemonstration/2.21.DataInspectionFromWorkbench.md</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G35" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.21.DataInspectionFromWorkbench.md</v>
+        <v>2.22.CoordinateSystemTransformation.md</v>
       </c>
       <c r="H35" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.11.DataInspectionFromWorkbench.md</v>
+        <v>DesktopBasic2Transformation/2.12.CoordinateSystemTransformation.md</v>
       </c>
       <c r="I35" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.21.DataInspectionFromWorkbench.md</v>
+        <v>CADGIS2LabDemonstration/2.22.CoordinateSystemTransformation.md</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>54</v>
-      </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="G36" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.22.CoordinateSystemTransformation.md</v>
+        <v>3.00.LabExercises.md</v>
       </c>
       <c r="H36" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.12.CoordinateSystemTransformation.md</v>
+        <v/>
       </c>
       <c r="I36" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.22.CoordinateSystemTransformation.md</v>
+        <v>CADGIS3LabExercises/3.00.LabExercises.md</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G37" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>3.00.LabExercises.md</v>
+        <v>3.01.GettingStartedWithFMEDesktop.md</v>
       </c>
       <c r="H37" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2291,403 +2289,403 @@
       </c>
       <c r="I37" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.00.LabExercises.md</v>
+        <v>CADGIS3LabExercises/3.01.GettingStartedWithFMEDesktop.md</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B38" t="s">
-        <v>95</v>
+      <c r="A38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G38" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.01.GettingStartedWithFMEDesktop.md</v>
+        <f t="shared" ref="G38:G56" si="3">IF(ISBLANK(A38),C38&amp;"."&amp;E38&amp;"."&amp;B38&amp;".md",C38&amp;"."&amp;E38&amp;"."&amp;RIGHT(B38,LEN(B38)-2))</f>
+        <v>3.02.Exercise1.md</v>
       </c>
       <c r="H38" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>DesktopBasic1Basics/1.Exercise1.md</v>
       </c>
       <c r="I38" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.01.GettingStartedWithFMEDesktop.md</v>
+        <v>CADGIS3LabExercises/3.02.Exercise1.md</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G39" s="2" t="str">
-        <f t="shared" ref="G38:G57" si="3">IF(ISBLANK(A39),C39&amp;"."&amp;E39&amp;"."&amp;B39&amp;".md",C39&amp;"."&amp;E39&amp;"."&amp;RIGHT(B39,LEN(B39)-2))</f>
-        <v>3.02.Exercise1.md</v>
+        <f t="shared" si="3"/>
+        <v>3.03.Exercise2.md</v>
       </c>
       <c r="H39" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.Exercise1.md</v>
+        <v>DesktopBasic1Basics/1.Exercise2.md</v>
       </c>
       <c r="I39" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.02.Exercise1.md</v>
+        <v>CADGIS3LabExercises/3.03.Exercise2.md</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.03.Exercise2.md</v>
+        <v>3.04.Exercise3.md</v>
       </c>
       <c r="H40" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.Exercise2.md</v>
+        <v>DesktopBasic1Basics/1.Exercise3.md</v>
       </c>
       <c r="I40" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.03.Exercise2.md</v>
+        <v>CADGIS3LabExercises/3.04.Exercise3.md</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G41" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.04.Exercise3.md</v>
+        <v>3.05.Exercise4.md</v>
       </c>
       <c r="H41" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.Exercise3.md</v>
+        <v>DesktopBasic1Basics/1.Exercise4.md</v>
       </c>
       <c r="I41" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.04.Exercise3.md</v>
+        <v>CADGIS3LabExercises/3.05.Exercise4.md</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.05.Exercise4.md</v>
-      </c>
-      <c r="H42" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.Exercise4.md</v>
+        <v>3.06.DataTransformation.md</v>
       </c>
       <c r="I42" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.05.Exercise4.md</v>
+        <v>CADGIS3LabExercises/3.06.DataTransformation.md</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1" t="s">
-        <v>91</v>
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" t="s">
+        <v>61</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G43" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.06.DataTransformation.md</v>
+        <v>3.07.Exercise1.md</v>
+      </c>
+      <c r="H43" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>DesktopBasic2Transformation/2.Exercise1.md</v>
       </c>
       <c r="I43" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.06.DataTransformation.md</v>
+        <v>CADGIS3LabExercises/3.07.Exercise1.md</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G44" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.07.Exercise1.md</v>
+        <v>3.08.Exercise2.md</v>
       </c>
       <c r="H44" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.Exercise1.md</v>
+        <v>DesktopBasic2Transformation/2.Exercise2.md</v>
       </c>
       <c r="I44" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.07.Exercise1.md</v>
+        <v>CADGIS3LabExercises/3.08.Exercise2.md</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G45" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.08.Exercise2.md</v>
+        <v>3.09.Exercise3.md</v>
       </c>
       <c r="H45" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.Exercise2.md</v>
+        <v>DesktopBasic2Transformation/2.Exercise3.md</v>
       </c>
       <c r="I45" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.08.Exercise2.md</v>
+        <v>CADGIS3LabExercises/3.09.Exercise3.md</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G46" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.09.Exercise3.md</v>
+        <v>3.10.Exercise4.md</v>
       </c>
       <c r="H46" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.Exercise3.md</v>
+        <v>DesktopBasic2Transformation/2.Exercise4.md</v>
       </c>
       <c r="I46" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.09.Exercise3.md</v>
+        <v>CADGIS3LabExercises/3.10.Exercise4.md</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G47" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.10.Exercise4.md</v>
+        <v>3.11.Exercise5.md</v>
       </c>
       <c r="H47" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.Exercise4.md</v>
+        <v>DesktopBasic2Transformation/2.Exercise5.md</v>
       </c>
       <c r="I47" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.10.Exercise4.md</v>
+        <v>CADGIS3LabExercises/3.11.Exercise5.md</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G48" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.11.Exercise5.md</v>
+        <v>3.12.Exercise6.md</v>
       </c>
       <c r="H48" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.Exercise5.md</v>
+        <v>DesktopBasic2Transformation/2.Exercise6.md</v>
       </c>
       <c r="I48" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.11.Exercise5.md</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>54</v>
-      </c>
+        <v>CADGIS3LabExercises/3.12.Exercise6.md</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G49" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.12.Exercise6.md</v>
+        <v>3.13.GettingStartedwithAutoCAD.md</v>
       </c>
       <c r="H49" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.Exercise6.md</v>
+        <v/>
       </c>
       <c r="I49" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.12.Exercise6.md</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+        <v>CADGIS3LabExercises/3.13.GettingStartedwithAutoCAD.md</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G50" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.13.GettingStartedwithAutoCAD.md</v>
+        <v>3.14.GroupingEntitiesInDWG.md</v>
       </c>
       <c r="H50" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2695,28 +2693,28 @@
       </c>
       <c r="I50" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.13.GettingStartedwithAutoCAD.md</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+        <v>CADGIS3LabExercises/3.14.GroupingEntitiesInDWG.md</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G51" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.14.GroupingEntitiesInDWG.md</v>
+        <v>3.15.HandlingBlocksInDWG.md</v>
       </c>
       <c r="H51" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2724,28 +2722,28 @@
       </c>
       <c r="I51" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.14.GroupingEntitiesInDWG.md</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+        <v>CADGIS3LabExercises/3.15.HandlingBlocksInDWG.md</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G52" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.15.HandlingBlocksInDWG.md</v>
+        <v>3.16.DWGToDGN.md</v>
       </c>
       <c r="H52" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2753,28 +2751,28 @@
       </c>
       <c r="I52" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.15.HandlingBlocksInDWG.md</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+        <v>CADGIS3LabExercises/3.16.DWGToDGN.md</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G53" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.16.DWGToDGN.md</v>
+        <v>3.17.SHPToDWG.md</v>
       </c>
       <c r="H53" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2782,28 +2780,28 @@
       </c>
       <c r="I53" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.16.DWGToDGN.md</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+        <v>CADGIS3LabExercises/3.17.SHPToDWG.md</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G54" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.17.SHPToDWG.md</v>
+        <v>3.18.ExplodingBlockEntitiesInDWG.md</v>
       </c>
       <c r="H54" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2811,28 +2809,28 @@
       </c>
       <c r="I54" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.17.SHPToDWG.md</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+        <v>CADGIS3LabExercises/3.18.ExplodingBlockEntitiesInDWG.md</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G55" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.18.ExplodingBlockEntitiesInDWG.md</v>
+        <v>3.19.PreservingBlockEntitiesInDWG.md</v>
       </c>
       <c r="H55" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2840,63 +2838,34 @@
       </c>
       <c r="I55" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.18.ExplodingBlockEntitiesInDWG.md</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+        <v>CADGIS3LabExercises/3.19.PreservingBlockEntitiesInDWG.md</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G56" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.19.PreservingBlockEntitiesInDWG.md</v>
+        <v>3.20.LabQuestions.md</v>
       </c>
       <c r="H56" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I56" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.19.PreservingBlockEntitiesInDWG.md</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B57" t="s">
-        <v>92</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G57" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>3.20.LabQuestions.md</v>
-      </c>
-      <c r="H57" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I57" s="2" t="str">
         <f t="shared" si="2"/>
         <v>CADGIS3LabExercises/3.20.LabQuestions.md</v>
       </c>
@@ -2911,14 +2880,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="5" width="8.7265625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1">
         <v>0</v>
@@ -2927,10 +2899,10 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="str">
         <f>IF(ISBLANK(A1),C1&amp;"."&amp;E1&amp;"."&amp;B1&amp;".md",C1&amp;"."&amp;E1&amp;"."&amp;RIGHT(B1,LEN(B1)-5))</f>
@@ -2948,49 +2920,49 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G2" s="2" t="str">
-        <f t="shared" ref="G2:G37" si="0">IF(ISBLANK(A2),C2&amp;"."&amp;E2&amp;"."&amp;B2&amp;".md",C2&amp;"."&amp;E2&amp;"."&amp;RIGHT(B2,LEN(B2)-5))</f>
+        <f t="shared" ref="G2:G36" si="0">IF(ISBLANK(A2),C2&amp;"."&amp;E2&amp;"."&amp;B2&amp;".md",C2&amp;"."&amp;E2&amp;"."&amp;RIGHT(B2,LEN(B2)-5))</f>
         <v>0.01.CourseOverview.md</v>
       </c>
       <c r="H2" s="2" t="str">
-        <f t="shared" ref="H2:H56" si="1">IF(ISBLANK(A2),"",A2&amp;"/"&amp;B2)</f>
+        <f t="shared" ref="H2:H55" si="1">IF(ISBLANK(A2),"",A2&amp;"/"&amp;B2)</f>
         <v/>
       </c>
       <c r="I2" s="2" t="str">
-        <f t="shared" ref="I2:I56" si="2">F2&amp;"/"&amp;G2</f>
+        <f t="shared" ref="I2:I55" si="2">F2&amp;"/"&amp;G2</f>
         <v>CADGIS0About/0.01.CourseOverview.md</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G3" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3008,19 +2980,19 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3028,26 +3000,26 @@
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="str">
-        <f>F4&amp;"/"&amp;G4</f>
+        <f t="shared" si="2"/>
         <v>CADGIS1Lecture/1.00.Lecture.md</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3057,982 +3029,984 @@
         <f>IF(ISBLANK(A5),"",A5&amp;"/"&amp;B4)</f>
         <v/>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>CADGIS1Lecture/1.01.DataIntegration.md</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1.02.WhyFME.md</v>
+        <v>1.02.WhatIsFME.md</v>
       </c>
       <c r="H6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>DesktopBasic1Basics/1.01.WhatIsFME.md</v>
       </c>
       <c r="I6" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS1Lecture/1.02.WhyFME.md</v>
+        <v>CADGIS1Lecture/1.02.WhatIsFME.md</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1.03.WhatIsFME.md</v>
+        <v>1.03.DataTransformation.md</v>
       </c>
       <c r="H7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.01.WhatIsFME.md</v>
+        <v>DesktopBasic2Transformation/2.00.DataTransformation.md</v>
       </c>
       <c r="I7" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS1Lecture/1.03.WhatIsFME.md</v>
+        <v>CADGIS1Lecture/1.03.DataTransformation.md</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1.04.DataTransformation.md</v>
+        <v>1.04.WhatIsDataTransformation.md</v>
       </c>
       <c r="H8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.00.DataTransformation.md</v>
+        <v>DesktopBasic2Transformation/2.01.WhatIsDataTransformation.md</v>
       </c>
       <c r="I8" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS1Lecture/1.04.DataTransformation.md</v>
+        <v>CADGIS1Lecture/1.04.WhatIsDataTransformation.md</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1.05.WhatIsDataTransformation.md</v>
+        <v>1.05.StructuralTransformation.md</v>
       </c>
       <c r="H9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.01.WhatIsDataTransformation.md</v>
+        <v>DesktopBasic2Transformation/2.02.StructuralTransformation.md</v>
       </c>
       <c r="I9" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS1Lecture/1.05.WhatIsDataTransformation.md</v>
+        <v>CADGIS1Lecture/1.05.StructuralTransformation.md</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1.06.StructuralTransformation.md</v>
+        <v>1.06.SchemaEditing.md</v>
       </c>
       <c r="H10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.02.StructuralTransformation.md</v>
+        <v>DesktopBasic2Transformation/2.03.SchemaEditing.md</v>
       </c>
       <c r="I10" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS1Lecture/1.06.StructuralTransformation.md</v>
+        <v>CADGIS1Lecture/1.06.SchemaEditing.md</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1.07.SchemaEditing.md</v>
+        <v>1.07.SchemaMapping.md</v>
       </c>
       <c r="H11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.03.SchemaEditing.md</v>
+        <v>DesktopBasic2Transformation/2.04.SchemaMapping.md</v>
       </c>
       <c r="I11" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS1Lecture/1.07.SchemaEditing.md</v>
+        <v>CADGIS1Lecture/1.07.SchemaMapping.md</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>54</v>
-      </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="G12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1.08.SchemaMapping.md</v>
+        <v>2.00.LabDemonstration.md</v>
       </c>
       <c r="H12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.04.SchemaMapping.md</v>
+        <v/>
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS1Lecture/1.08.SchemaMapping.md</v>
+        <v>CADGIS2LabDemonstration/2.00.LabDemonstration.md</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>90</v>
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.00.LabDemonstration.md</v>
+        <v>2.01.FMEDesktopComponents.md</v>
       </c>
       <c r="H13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>DesktopBasic1Basics/1.02.FMEDesktopComponents.md</v>
       </c>
       <c r="I13" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.00.LabDemonstration.md</v>
+        <v>CADGIS2LabDemonstration/2.01.FMEDesktopComponents.md</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.01.FMEDesktopComponents.md</v>
+        <v>2.02.IntroductionToWorkbench.md</v>
       </c>
       <c r="H14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.02.FMEDesktopComponents.md</v>
+        <v>DesktopBasic1Basics/1.03.IntroductionToWorkbench.md</v>
       </c>
       <c r="I14" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.01.FMEDesktopComponents.md</v>
+        <v>CADGIS2LabDemonstration/2.02.IntroductionToWorkbench.md</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.02.IntroductionToWorkbench.md</v>
+        <v>2.03.WindowControl.md</v>
       </c>
       <c r="H15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.03.IntroductionToWorkbench.md</v>
+        <v>DesktopBasic1Basics/1.04.WindowControl.md</v>
       </c>
       <c r="I15" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.02.IntroductionToWorkbench.md</v>
+        <v>CADGIS2LabDemonstration/2.03.WindowControl.md</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.03.WindowControl.md</v>
+        <v>2.04.CreatingATranslation.md</v>
       </c>
       <c r="H16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.04.WindowControl.md</v>
+        <v>DesktopBasic1Basics/1.05.CreatingATranslation.md</v>
       </c>
       <c r="I16" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.03.WindowControl.md</v>
+        <v>CADGIS2LabDemonstration/2.04.CreatingATranslation.md</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.04.CreatingATranslation.md</v>
+        <v>2.05.TheNewWorkspace.md</v>
       </c>
       <c r="H17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.05.CreatingATranslation.md</v>
+        <v>DesktopBasic1Basics/1.06.TheNewWorkspace.md</v>
       </c>
       <c r="I17" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.04.CreatingATranslation.md</v>
+        <v>CADGIS2LabDemonstration/2.05.TheNewWorkspace.md</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.05.TheNewWorkspace.md</v>
+        <v>2.06.RunningTheWorkspace.md</v>
       </c>
       <c r="H18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.06.TheNewWorkspace.md</v>
+        <v>DesktopBasic1Basics/1.07.RunningTheWorkspace.md</v>
       </c>
       <c r="I18" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.05.TheNewWorkspace.md</v>
+        <v>CADGIS2LabDemonstration/2.06.RunningTheWorkspace.md</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.06.RunningTheWorkspace.md</v>
+        <v>2.07.WhatIsDataInspection.md</v>
       </c>
       <c r="H19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.07.RunningTheWorkspace.md</v>
+        <v>DesktopBasic1Basics/1.08.WhatIsDataInspection.md</v>
       </c>
       <c r="I19" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.06.RunningTheWorkspace.md</v>
+        <v>CADGIS2LabDemonstration/2.07.WhatIsDataInspection.md</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.07.WhatIsDataInspection.md</v>
+        <v>2.08.IntroductionToDataInspector.md</v>
       </c>
       <c r="H20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.08.WhatIsDataInspection.md</v>
+        <v>DesktopBasic1Basics/1.09.IntroductionToDataInspector.md</v>
       </c>
       <c r="I20" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.07.WhatIsDataInspection.md</v>
+        <v>CADGIS2LabDemonstration/2.08.IntroductionToDataInspector.md</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.08.IntroductionToDataInspector.md</v>
+        <v>2.09.ViewingData.md</v>
       </c>
       <c r="H21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.09.IntroductionToDataInspector.md</v>
+        <v>DesktopBasic1Basics/1.10.ViewingData.md</v>
       </c>
       <c r="I21" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.08.IntroductionToDataInspector.md</v>
+        <v>CADGIS2LabDemonstration/2.09.ViewingData.md</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.09.ViewingData.md</v>
+        <v>2.10.QueryingData.md</v>
       </c>
       <c r="H22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.10.ViewingData.md</v>
+        <v>DesktopBasic1Basics/1.11.QueryingData.md</v>
       </c>
       <c r="I22" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.09.ViewingData.md</v>
+        <v>CADGIS2LabDemonstration/2.10.QueryingData.md</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.10.QueryingData.md</v>
+        <v>2.11.DataInspectorDisplayControl.md</v>
       </c>
       <c r="H23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.11.QueryingData.md</v>
+        <v>DesktopBasic1Basics/1.12.DataInspectorDisplayControl.md</v>
       </c>
       <c r="I23" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.10.QueryingData.md</v>
+        <v>CADGIS2LabDemonstration/2.11.DataInspectorDisplayControl.md</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.11.DataInspectorDisplayControl.md</v>
+        <v>2.12.BackgroundMaps.md</v>
       </c>
       <c r="H24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.12.DataInspectorDisplayControl.md</v>
+        <v>DesktopBasic1Basics/1.13.BackgroundMaps.md</v>
       </c>
       <c r="I24" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.11.DataInspectorDisplayControl.md</v>
+        <v>CADGIS2LabDemonstration/2.12.BackgroundMaps.md</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.12.BackgroundMaps.md</v>
+        <v>2.13.ReaderParameters.md</v>
       </c>
       <c r="H25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.13.BackgroundMaps.md</v>
+        <v>DesktopBasic1Basics/1.14.ReaderParameters.md</v>
       </c>
       <c r="I25" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.12.BackgroundMaps.md</v>
+        <v>CADGIS2LabDemonstration/2.13.ReaderParameters.md</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.13.ReaderParameters.md</v>
+        <v>2.14.WriterParameters.md</v>
       </c>
       <c r="H26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.14.ReaderParameters.md</v>
+        <v>DesktopBasic1Basics/1.15.WriterParameters.md</v>
       </c>
       <c r="I26" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.13.ReaderParameters.md</v>
+        <v>CADGIS2LabDemonstration/2.14.WriterParameters.md</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>12</v>
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>42</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.14.WriterParameters.md</v>
+        <v>2.15.TransformationWithTransformers.md</v>
       </c>
       <c r="H27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.15.WriterParameters.md</v>
+        <v>DesktopBasic2Transformation/2.05.TransformationWithTransformers.md</v>
       </c>
       <c r="I27" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.14.WriterParameters.md</v>
+        <v>CADGIS2LabDemonstration/2.15.TransformationWithTransformers.md</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.15.TransformationWithTransformers.md</v>
+        <v>2.16.ContentTransformation.md</v>
       </c>
       <c r="H28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.05.TransformationWithTransformers.md</v>
+        <v>DesktopBasic2Transformation/2.06.ContentTransformation.md</v>
       </c>
       <c r="I28" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.15.TransformationWithTransformers.md</v>
+        <v>CADGIS2LabDemonstration/2.16.ContentTransformation.md</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.16.ContentTransformation.md</v>
+        <v>2.17.TransformersInSeries.md</v>
       </c>
       <c r="H29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.06.ContentTransformation.md</v>
+        <v>DesktopBasic2Transformation/2.07.TransformersInSeries.md</v>
       </c>
       <c r="I29" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.16.ContentTransformation.md</v>
+        <v>CADGIS2LabDemonstration/2.17.TransformersInSeries.md</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.17.TransformersInSeries.md</v>
+        <v>2.18.FeatureCounts.md</v>
       </c>
       <c r="H30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.07.TransformersInSeries.md</v>
+        <v>DesktopBasic2Transformation/2.08.FeatureCounts.md</v>
       </c>
       <c r="I30" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.17.TransformersInSeries.md</v>
+        <v>CADGIS2LabDemonstration/2.18.FeatureCounts.md</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.18.FeatureCounts.md</v>
+        <v>2.19.TransformersInParallel.md</v>
       </c>
       <c r="H31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.08.FeatureCounts.md</v>
+        <v>DesktopBasic2Transformation/2.09.TransformersInParallel.md</v>
       </c>
       <c r="I31" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.18.FeatureCounts.md</v>
+        <v>CADGIS2LabDemonstration/2.19.TransformersInParallel.md</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.19.TransformersInParallel.md</v>
+        <v>2.20.GroupByProcessing.md</v>
       </c>
       <c r="H32" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.09.TransformersInParallel.md</v>
+        <v>DesktopBasic2Transformation/2.10.GroupByProcessing.md</v>
       </c>
       <c r="I32" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.19.TransformersInParallel.md</v>
+        <v>CADGIS2LabDemonstration/2.20.GroupByProcessing.md</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G33" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.20.GroupByProcessing.md</v>
+        <v>2.21.DataInspectionFromWorkbench.md</v>
       </c>
       <c r="H33" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.10.GroupByProcessing.md</v>
+        <v>DesktopBasic2Transformation/2.11.DataInspectionFromWorkbench.md</v>
       </c>
       <c r="I33" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.20.GroupByProcessing.md</v>
+        <v>CADGIS2LabDemonstration/2.21.DataInspectionFromWorkbench.md</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G34" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.21.DataInspectionFromWorkbench.md</v>
+        <v>2.22.CoordinateSystemTransformation.md</v>
       </c>
       <c r="H34" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.11.DataInspectionFromWorkbench.md</v>
+        <v>DesktopBasic2Transformation/2.12.CoordinateSystemTransformation.md</v>
       </c>
       <c r="I34" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.21.DataInspectionFromWorkbench.md</v>
+        <v>CADGIS2LabDemonstration/2.22.CoordinateSystemTransformation.md</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>54</v>
-      </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="G35" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>2.22.CoordinateSystemTransformation.md</v>
+        <v>3.00.LabExercises.md</v>
       </c>
       <c r="H35" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.12.CoordinateSystemTransformation.md</v>
+        <v/>
       </c>
       <c r="I35" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS2LabDemonstration/2.22.CoordinateSystemTransformation.md</v>
+        <v>CADGIS3LabExercises/3.00.LabExercises.md</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G36" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>3.00.LabExercises.md</v>
+        <v>3.01.GettingStartedWithFMEDesktop.md</v>
       </c>
       <c r="H36" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4040,404 +4014,404 @@
       </c>
       <c r="I36" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.00.LabExercises.md</v>
+        <v>CADGIS3LabExercises/3.01.GettingStartedWithFMEDesktop.md</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B37" t="s">
-        <v>95</v>
+      <c r="A37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G37" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.01.GettingStartedWithFMEDesktop.md</v>
+        <f t="shared" ref="G37:G55" si="3">IF(ISBLANK(A37),C37&amp;"."&amp;E37&amp;"."&amp;B37&amp;".md",C37&amp;"."&amp;E37&amp;"."&amp;RIGHT(B37,LEN(B37)-2))</f>
+        <v>3.02.Exercise1.md</v>
       </c>
       <c r="H37" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>DesktopBasic1Basics/1.Exercise1.md</v>
       </c>
       <c r="I37" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.01.GettingStartedWithFMEDesktop.md</v>
+        <v>CADGIS3LabExercises/3.02.Exercise1.md</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G38" s="2" t="str">
-        <f t="shared" ref="G38:G56" si="3">IF(ISBLANK(A38),C38&amp;"."&amp;E38&amp;"."&amp;B38&amp;".md",C38&amp;"."&amp;E38&amp;"."&amp;RIGHT(B38,LEN(B38)-2))</f>
-        <v>3.02.Exercise1.md</v>
+        <f t="shared" si="3"/>
+        <v>3.03.Exercise2.md</v>
       </c>
       <c r="H38" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.Exercise1.md</v>
+        <v>DesktopBasic1Basics/1.Exercise2.md</v>
       </c>
       <c r="I38" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.02.Exercise1.md</v>
+        <v>CADGIS3LabExercises/3.03.Exercise2.md</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G39" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.03.Exercise2.md</v>
+        <v>3.04.Exercise3.md</v>
       </c>
       <c r="H39" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.Exercise2.md</v>
+        <v>DesktopBasic1Basics/1.Exercise3.md</v>
       </c>
       <c r="I39" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.03.Exercise2.md</v>
+        <v>CADGIS3LabExercises/3.04.Exercise3.md</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.04.Exercise3.md</v>
+        <v>3.05.Exercise4.md</v>
       </c>
       <c r="H40" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.Exercise3.md</v>
+        <v>DesktopBasic1Basics/1.Exercise4.md</v>
       </c>
       <c r="I40" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.04.Exercise3.md</v>
+        <v>CADGIS3LabExercises/3.05.Exercise4.md</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G41" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.05.Exercise4.md</v>
-      </c>
-      <c r="H41" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>DesktopBasic1Basics/1.Exercise4.md</v>
-      </c>
+        <v>3.06.DataTransformation.md</v>
+      </c>
+      <c r="H41" s="2"/>
       <c r="I41" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.05.Exercise4.md</v>
+        <v>CADGIS3LabExercises/3.06.DataTransformation.md</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1" t="s">
-        <v>91</v>
+      <c r="A42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" t="s">
+        <v>61</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.06.DataTransformation.md</v>
-      </c>
-      <c r="H42" s="2"/>
+        <v>3.07.Exercise1.md</v>
+      </c>
+      <c r="H42" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>DesktopBasic2Transformation/2.Exercise1.md</v>
+      </c>
       <c r="I42" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.06.DataTransformation.md</v>
+        <v>CADGIS3LabExercises/3.07.Exercise1.md</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G43" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.07.Exercise1.md</v>
+        <v>3.08.Exercise2.md</v>
       </c>
       <c r="H43" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.Exercise1.md</v>
+        <v>DesktopBasic2Transformation/2.Exercise2.md</v>
       </c>
       <c r="I43" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.07.Exercise1.md</v>
+        <v>CADGIS3LabExercises/3.08.Exercise2.md</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G44" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.08.Exercise2.md</v>
+        <v>3.09.Exercise3.md</v>
       </c>
       <c r="H44" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.Exercise2.md</v>
+        <v>DesktopBasic2Transformation/2.Exercise3.md</v>
       </c>
       <c r="I44" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.08.Exercise2.md</v>
+        <v>CADGIS3LabExercises/3.09.Exercise3.md</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G45" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.09.Exercise3.md</v>
+        <v>3.10.Exercise4.md</v>
       </c>
       <c r="H45" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.Exercise3.md</v>
+        <v>DesktopBasic2Transformation/2.Exercise4.md</v>
       </c>
       <c r="I45" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.09.Exercise3.md</v>
+        <v>CADGIS3LabExercises/3.10.Exercise4.md</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G46" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.10.Exercise4.md</v>
+        <v>3.11.Exercise5.md</v>
       </c>
       <c r="H46" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.Exercise4.md</v>
+        <v>DesktopBasic2Transformation/2.Exercise5.md</v>
       </c>
       <c r="I46" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.10.Exercise4.md</v>
+        <v>CADGIS3LabExercises/3.11.Exercise5.md</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G47" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.11.Exercise5.md</v>
+        <v>3.12.Exercise6.md</v>
       </c>
       <c r="H47" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.Exercise5.md</v>
+        <v>DesktopBasic2Transformation/2.Exercise6.md</v>
       </c>
       <c r="I47" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.11.Exercise5.md</v>
+        <v>CADGIS3LabExercises/3.12.Exercise6.md</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>54</v>
-      </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G48" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.12.Exercise6.md</v>
+        <v>3.13.GettingStartedwithAutoCAD.md</v>
       </c>
       <c r="H48" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DesktopBasic2Transformation/2.Exercise6.md</v>
+        <v/>
       </c>
       <c r="I48" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.12.Exercise6.md</v>
+        <v>CADGIS3LabExercises/3.13.GettingStartedwithAutoCAD.md</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G49" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.13.GettingStartedwithAutoCAD.md</v>
+        <v>3.14.GroupingEntitiesInDWG.md</v>
       </c>
       <c r="H49" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4445,28 +4419,28 @@
       </c>
       <c r="I49" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.13.GettingStartedwithAutoCAD.md</v>
+        <v>CADGIS3LabExercises/3.14.GroupingEntitiesInDWG.md</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G50" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.14.GroupingEntitiesInDWG.md</v>
+        <v>3.15.HandlingBlocksInDWG.md</v>
       </c>
       <c r="H50" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4474,28 +4448,28 @@
       </c>
       <c r="I50" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.14.GroupingEntitiesInDWG.md</v>
+        <v>CADGIS3LabExercises/3.15.HandlingBlocksInDWG.md</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G51" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.15.HandlingBlocksInDWG.md</v>
+        <v>3.16.DWGToDGN.md</v>
       </c>
       <c r="H51" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4503,28 +4477,28 @@
       </c>
       <c r="I51" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.15.HandlingBlocksInDWG.md</v>
+        <v>CADGIS3LabExercises/3.16.DWGToDGN.md</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G52" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.16.DWGToDGN.md</v>
+        <v>3.17.SHPToDWG.md</v>
       </c>
       <c r="H52" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4532,28 +4506,28 @@
       </c>
       <c r="I52" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.16.DWGToDGN.md</v>
+        <v>CADGIS3LabExercises/3.17.SHPToDWG.md</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G53" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.17.SHPToDWG.md</v>
+        <v>3.18.ExplodingBlockEntitiesInDWG.md</v>
       </c>
       <c r="H53" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4561,28 +4535,28 @@
       </c>
       <c r="I53" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.17.SHPToDWG.md</v>
+        <v>CADGIS3LabExercises/3.18.ExplodingBlockEntitiesInDWG.md</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G54" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.18.ExplodingBlockEntitiesInDWG.md</v>
+        <v>3.19.PreservingBlockEntitiesInDWG.md</v>
       </c>
       <c r="H54" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4590,28 +4564,28 @@
       </c>
       <c r="I54" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.18.ExplodingBlockEntitiesInDWG.md</v>
+        <v>CADGIS3LabExercises/3.19.PreservingBlockEntitiesInDWG.md</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G55" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3.19.PreservingBlockEntitiesInDWG.md</v>
+        <v>3.20.LabQuestions.md</v>
       </c>
       <c r="H55" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4619,39 +4593,17 @@
       </c>
       <c r="I55" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.19.PreservingBlockEntitiesInDWG.md</v>
+        <v>CADGIS3LabExercises/3.20.LabQuestions.md</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B56" t="s">
-        <v>92</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G56" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>3.20.LabQuestions.md</v>
-      </c>
-      <c r="H56" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I56" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>CADGIS3LabExercises/3.20.LabQuestions.md</v>
-      </c>
+      <c r="F56" s="1"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating python to download KC articles
</commit_message>
<xml_diff>
--- a/chapters.xlsx
+++ b/chapters.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="97">
   <si>
     <t>1.03.IntroductionToWorkbench.md</t>
   </si>
@@ -286,13 +286,37 @@
   </si>
   <si>
     <t>ModuleResources</t>
+  </si>
+  <si>
+    <t>https://knowledge.safe.com/content/kbentry/22435/getting-started-with-autocad-and-fme-reader-parame.html</t>
+  </si>
+  <si>
+    <t>https://knowledge.safe.com/articles/27244/viewing-and-inspecting-autocad-dwg-data-handling-b.html</t>
+  </si>
+  <si>
+    <t>https://knowledge.safe.com/articles/22968/getting-started-with-autocad.html</t>
+  </si>
+  <si>
+    <t>https://knowledge.safe.com/articles/1470/how-to-convert-dwg-to-dgn-autocad-to-microstation.html</t>
+  </si>
+  <si>
+    <t>https://knowledge.safe.com/articles/18703/how-to-convert-shp-to-dwg-esri-shapefile-to-autoca.html</t>
+  </si>
+  <si>
+    <t>https://knowledge.safe.com/articles/27245/basic-dwg-block-handling-example-exploding-block-e.html</t>
+  </si>
+  <si>
+    <t>https://knowledge.safe.com/articles/18737/tutorial-getting-started-with-autocad-and-fme.html</t>
+  </si>
+  <si>
+    <t>kc_link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,6 +451,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -725,7 +757,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -768,13 +800,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -808,6 +842,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1094,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1111,7 +1146,7 @@
     <col min="9" max="9" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -1139,8 +1174,11 @@
       <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>80</v>
@@ -1170,7 +1208,7 @@
         <v>CADGIS0About/0.00.AboutThisDocument.md</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>87</v>
@@ -1200,7 +1238,7 @@
         <v>CADGIS0About/0.01.ModuleOverview.md</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>88</v>
@@ -1230,7 +1268,7 @@
         <v>CADGIS0About/0.02.ModuleResources.md</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>63</v>
@@ -1256,7 +1294,7 @@
         <v>CADGIS1Lecture/1.00.Lecture.md</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>84</v>
       </c>
@@ -1277,7 +1315,7 @@
         <v>1.01.CADGISIntegration.md</v>
       </c>
       <c r="H6" s="2" t="str">
-        <f t="shared" ref="H6:H44" si="2">IF(ISBLANK(A6),"",A6&amp;"/"&amp;B6)</f>
+        <f t="shared" ref="H6:H45" si="2">IF(ISBLANK(A6),"",A6&amp;"/"&amp;B6)</f>
         <v/>
       </c>
       <c r="I6" s="2" t="str">
@@ -1285,7 +1323,7 @@
         <v>CADGIS1Lecture/1.01.CADGISIntegration.md</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1317,7 +1355,7 @@
         <v>CADGIS1Lecture/1.02.WhatIsFME.md</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -1349,7 +1387,7 @@
         <v>CADGIS1Lecture/1.03.DataTransformation.md</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1381,7 +1419,7 @@
         <v>CADGIS1Lecture/1.04.WhatIsDataTransformation.md</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>71</v>
       </c>
@@ -1410,7 +1448,7 @@
         <v>CADGIS2LabDemonstration/2.00.LabDemonstration.md</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1442,7 +1480,7 @@
         <v>CADGIS2LabDemonstration/2.01.FMEDesktopComponents.md</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1474,7 +1512,7 @@
         <v>CADGIS2LabDemonstration/2.02.IntroductionToWorkbench.md</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1506,7 +1544,7 @@
         <v>CADGIS2LabDemonstration/2.03.WindowControl.md</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1538,7 +1576,7 @@
         <v>CADGIS2LabDemonstration/2.04.CreatingATranslation.md</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1570,7 +1608,7 @@
         <v>CADGIS2LabDemonstration/2.05.TheNewWorkspace.md</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -2114,7 +2152,7 @@
         <v>CADGIS2LabDemonstration/2.22.TransformersInParallel.md</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -2146,7 +2184,7 @@
         <v>CADGIS2LabDemonstration/2.23.GroupByProcessing.md</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -2178,7 +2216,7 @@
         <v>CADGIS2LabDemonstration/2.24.DataInspectionFromWorkbench.md</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -2210,7 +2248,7 @@
         <v>CADGIS2LabDemonstration/2.25.CoordinateSystemTransformation.md</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>64</v>
       </c>
@@ -2239,7 +2277,7 @@
         <v>CADGIS3LabExercises/3.00.LabExercises.md</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>65</v>
       </c>
@@ -2267,8 +2305,11 @@
         <f t="shared" si="1"/>
         <v>CADGIS3LabExercises/3.01.GettingStartedwithAutoCAD.md</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J37" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>67</v>
       </c>
@@ -2296,8 +2337,11 @@
         <f t="shared" si="1"/>
         <v>CADGIS3LabExercises/3.02.GroupingEntitiesInDWG.md</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J38" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>66</v>
       </c>
@@ -2325,8 +2369,11 @@
         <f t="shared" si="1"/>
         <v>CADGIS3LabExercises/3.03.HandlingBlocksInDWG.md</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J39" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>73</v>
       </c>
@@ -2354,8 +2401,11 @@
         <f t="shared" si="1"/>
         <v>CADGIS3LabExercises/3.04.DWGToDGN.md</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J40" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>74</v>
       </c>
@@ -2383,8 +2433,11 @@
         <f t="shared" si="1"/>
         <v>CADGIS3LabExercises/3.05.SHPToDWG.md</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J41" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>68</v>
       </c>
@@ -2412,8 +2465,11 @@
         <f t="shared" si="1"/>
         <v>CADGIS3LabExercises/3.06.ExplodingBlockEntitiesInDWG.md</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J42" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>69</v>
       </c>
@@ -2441,8 +2497,11 @@
         <f t="shared" si="1"/>
         <v>CADGIS3LabExercises/3.07.PreservingBlockEntitiesInDWG.md</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J43" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>86</v>
       </c>
@@ -2471,7 +2530,7 @@
         <v>CADGIS3LabExercises/3.08.CADGISScenario.md</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>72</v>
       </c>
@@ -2492,7 +2551,7 @@
         <v>3.09.LabQuestions.md</v>
       </c>
       <c r="H45" s="2" t="str">
-        <f>IF(ISBLANK(A44),"",A44&amp;"/"&amp;B45)</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I45" s="2" t="str">
@@ -2501,7 +2560,16 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J38" r:id="rId1"/>
+    <hyperlink ref="J39" r:id="rId2"/>
+    <hyperlink ref="J37" r:id="rId3"/>
+    <hyperlink ref="J40" r:id="rId4"/>
+    <hyperlink ref="J41" r:id="rId5"/>
+    <hyperlink ref="J42" r:id="rId6"/>
+    <hyperlink ref="J43" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>